<commit_message>
Writer and reader from json and to csv file added. all the needed files are inside the input folder. Calls analization added.
</commit_message>
<xml_diff>
--- a/AnalizeCalls/Call b analization.xlsx
+++ b/AnalizeCalls/Call b analization.xlsx
@@ -1,34 +1,90 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://msmailarielac-my.sharepoint.com/personal/yan_naigebav_msmail_ariel_ac_il/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yan-PC\PycharmProjects\Ex1\AnalizeCalls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67A34732-8C6E-4CD4-AB7E-1BF99FD4F713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5B68ED8-8435-4FA9-ACFC-74EC0E667E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calls_b" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="16">
   <si>
     <t>Elevator call</t>
+  </si>
+  <si>
+    <t>average source calls</t>
+  </si>
+  <si>
+    <t>average destination calls</t>
+  </si>
+  <si>
+    <t>"-10 to 0"</t>
+  </si>
+  <si>
+    <t>"0 to 10"</t>
+  </si>
+  <si>
+    <t>"10 to 20"</t>
+  </si>
+  <si>
+    <t>"20 to 30"</t>
+  </si>
+  <si>
+    <t>"30 to 40"</t>
+  </si>
+  <si>
+    <t>"40 to 50"</t>
+  </si>
+  <si>
+    <t>"50 to 60"</t>
+  </si>
+  <si>
+    <t>"60 to 70"</t>
+  </si>
+  <si>
+    <t>"70 to 80"</t>
+  </si>
+  <si>
+    <t>"80 to 90"</t>
+  </si>
+  <si>
+    <t>"90 to 100"</t>
+  </si>
+  <si>
+    <t>destination</t>
+  </si>
+  <si>
+    <t>calls</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6893,7 +6949,1072 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Source calls distribution </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IL">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-0B16-43AF-B7F9-2C32579C8914}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-0B16-43AF-B7F9-2C32579C8914}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-0B16-43AF-B7F9-2C32579C8914}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-0B16-43AF-B7F9-2C32579C8914}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-0B16-43AF-B7F9-2C32579C8914}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-0B16-43AF-B7F9-2C32579C8914}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-0B16-43AF-B7F9-2C32579C8914}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-0B16-43AF-B7F9-2C32579C8914}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-0B16-43AF-B7F9-2C32579C8914}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-0B16-43AF-B7F9-2C32579C8914}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-0B16-43AF-B7F9-2C32579C8914}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Calls_b!$I$7:$I$17</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>"-10 to 0"</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>"0 to 10"</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>"10 to 20"</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>"20 to 30"</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>"30 to 40"</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>"40 to 50"</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>"50 to 60"</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>"60 to 70"</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>"70 to 80"</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>"80 to 90"</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>"90 to 100"</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Calls_b!$J$7:$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D770-44C0-B6DA-66A9F69C3C52}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Destionation calls distribution</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-F907-4D72-8316-4222FDBA2EE7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-F907-4D72-8316-4222FDBA2EE7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-F907-4D72-8316-4222FDBA2EE7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-F907-4D72-8316-4222FDBA2EE7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-F907-4D72-8316-4222FDBA2EE7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-F907-4D72-8316-4222FDBA2EE7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-F907-4D72-8316-4222FDBA2EE7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-F907-4D72-8316-4222FDBA2EE7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-F907-4D72-8316-4222FDBA2EE7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-F907-4D72-8316-4222FDBA2EE7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-F907-4D72-8316-4222FDBA2EE7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Calls_b!$I$24:$I$34</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>"-10 to 0"</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>"0 to 10"</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>"10 to 20"</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>"20 to 30"</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>"30 to 40"</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>"40 to 50"</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>"50 to 60"</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>"60 to 70"</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>"70 to 80"</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>"80 to 90"</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>"90 to 100"</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Calls_b!$J$24:$J$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>503</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-416F-4ACC-A49D-624F8865EBB5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7449,18 +8570,1056 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
@@ -7482,6 +9641,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>100011</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D81AC9C8-3E24-49D8-B9D2-A702BABB088D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E79C1BD-C843-4CEA-95DD-FA18D06AA43B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7786,16 +10017,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" activeCellId="1" sqref="B1:B1048576 G1:G1048576"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7818,7 +10049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7841,8 +10072,14 @@
         <f>G1+1</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -7865,8 +10102,16 @@
         <f t="shared" ref="G3:G66" si="0">G2+1</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <f>AVERAGE(C:C)</f>
+        <v>20.826000000000001</v>
+      </c>
+      <c r="J3">
+        <f>AVERAGE(D:D)</f>
+        <v>18.591999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -7890,7 +10135,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -7914,7 +10159,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -7938,7 +10183,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -7961,8 +10206,15 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <f>COUNTIF(C:C,"&gt;=-10")-COUNTIF(C:C,"&gt;=0")</f>
+        <v>492</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -7985,8 +10237,15 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <f>ABS(COUNTIF(C:C,"&gt;=0")- COUNTIF(C:C,"&gt;=10"))</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -8009,8 +10268,15 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <f>ABS(COUNTIF(C:C,"&gt;=10")-COUNTIF(C:C,"&gt;=20"))</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -8033,8 +10299,15 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10">
+        <f>ABS(COUNTIF(C:C,"&gt;=20")-COUNTIF(C:C,"&gt;=30"))</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -8057,8 +10330,15 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11">
+        <f>ABS(COUNTIF(C:C,"&gt;=30")-COUNTIF(C:C,"&gt;=40"))</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -8081,8 +10361,15 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12">
+        <f>ABS(COUNTIF(C:C,"&gt;=40")-COUNTIF(C:C,"&gt;=50"))</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -8105,8 +10392,15 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13">
+        <f>ABS(COUNTIF(C:C,"&gt;=50")-COUNTIF(C:C,"&gt;=60"))</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -8129,8 +10423,15 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14">
+        <f>ABS(COUNTIF(C:C,"&gt;=60")-COUNTIF(C:C,"&gt;=70"))</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -8153,8 +10454,15 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15">
+        <f>ABS(COUNTIF(C:C,"&gt;=70")-COUNTIF(C:C,"&gt;=80"))</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -8177,8 +10485,15 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16">
+        <f>ABS(COUNTIF(C:C,"&gt;=80")-COUNTIF(C:C,"&gt;=90"))</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -8201,8 +10516,15 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17">
+        <f>ABS(COUNTIF(C:C,"&gt;=90")-COUNTIF(C:C,"&gt;=100"))</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -8226,7 +10548,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -8250,7 +10572,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -8274,7 +10596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -8298,7 +10620,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -8322,7 +10644,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -8345,8 +10667,14 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -8369,8 +10697,15 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <f>COUNTIF(D:D,"&gt;=-10")-COUNTIF(D:D,"&gt;=0")</f>
+        <v>503</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -8393,8 +10728,15 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25">
+        <f>COUNTIF(D:D,"&gt;=0")-COUNTIF(D:D,"&gt;=10")</f>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -8417,8 +10759,15 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>5</v>
+      </c>
+      <c r="J26">
+        <f>COUNTIF(D:D,"&gt;=10")-COUNTIF(D:D,"&gt;=20")</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -8441,8 +10790,15 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27">
+        <f>COUNTIF(D:D,"&gt;=20")-COUNTIF(D:D,"&gt;=30")</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -8465,8 +10821,15 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28">
+        <f>COUNTIF(D:D,"&gt;=30")-COUNTIF(D:D,"&gt;=40")</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -8489,8 +10852,15 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>8</v>
+      </c>
+      <c r="J29">
+        <f>COUNTIF(D:D,"&gt;=40")-COUNTIF(D:D,"&gt;=50")</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -8513,8 +10883,15 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30">
+        <f>COUNTIF(D:D,"&gt;=50")-COUNTIF(D:D,"&gt;=60")</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -8537,8 +10914,15 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J31">
+        <f>COUNTIF(D:D,"&gt;=60")-COUNTIF(D:D,"&gt;=70")</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -8561,8 +10945,15 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32">
+        <f>COUNTIF(D:D,"&gt;=70")-COUNTIF(D:D,"&gt;=80")</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -8585,8 +10976,15 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>12</v>
+      </c>
+      <c r="J33">
+        <f>COUNTIF(D:D,"&gt;=80")-COUNTIF(D:D,"&gt;=90")</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -8609,8 +11007,15 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>13</v>
+      </c>
+      <c r="J34">
+        <f>COUNTIF(D:D,"&gt;=90")-COUNTIF(D:D,"&gt;100")</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -8634,7 +11039,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -8658,7 +11063,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -8682,7 +11087,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -8706,7 +11111,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -8730,7 +11135,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -8754,7 +11159,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -8778,7 +11183,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -8802,7 +11207,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -8826,7 +11231,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -8850,7 +11255,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -8874,7 +11279,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -8898,7 +11303,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -8922,7 +11327,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -31801,6 +34206,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BCB8A3745F5D7347B3C87A03D1F53609" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="095b86974212203ed5becdbbce7fb174">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="decf5da3-6a3a-417a-802f-a7dc231907bc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="97c320c72ae3360f9eecbf23aa0ce659" ns3:_="">
     <xsd:import namespace="decf5da3-6a3a-417a-802f-a7dc231907bc"/>
@@ -31946,15 +34360,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -31962,6 +34367,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E66A504-B5D3-4C3B-8BC5-9E417B068FD2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF3035B-3095-4741-970E-765C7FD1AF97}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -31975,14 +34388,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E66A504-B5D3-4C3B-8BC5-9E417B068FD2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>